<commit_message>
Database Foundations Easy Practice Problems
</commit_message>
<xml_diff>
--- a/File Naming Tool.xlsx
+++ b/File Naming Tool.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Google Drive\LaunchSchool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Google Drive\LS\LaunchSchool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34F6A9D-3F4C-446A-A8BE-65CF01C8CB62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE800242-4B8A-4B48-8BF1-B5D21B575719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="4910" windowWidth="17330" windowHeight="11450" xr2:uid="{C3B8B670-4DBA-4CAF-91B9-F79D6235264A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{C3B8B670-4DBA-4CAF-91B9-F79D6235264A}"/>
   </bookViews>
   <sheets>
     <sheet name="RB101 Small Problems" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="34">
   <si>
     <t>1_</t>
   </si>
@@ -101,157 +101,40 @@
     <t>Debugging</t>
   </si>
   <si>
-    <t>Enumerable Class Creation</t>
-  </si>
-  <si>
     <t>Easy Testing</t>
   </si>
   <si>
     <t>Medium 2: Testing</t>
   </si>
   <si>
-    <t>Optional Blocks</t>
-  </si>
-  <si>
-    <t>Find Missing Numbers</t>
-  </si>
-  <si>
-    <t>Divisors</t>
-  </si>
-  <si>
-    <t>Encrypted Pioneers</t>
-  </si>
-  <si>
-    <t>Iterators: True for Any?</t>
-  </si>
-  <si>
-    <t>Iterators: True for All?</t>
-  </si>
-  <si>
-    <t>Iterators: True for None?</t>
-  </si>
-  <si>
-    <t>Iterators: True for One?</t>
-  </si>
-  <si>
-    <t>Count Items</t>
-  </si>
-  <si>
-    <t>From-To-Step Sequence Generator</t>
-  </si>
-  <si>
-    <t>Zipper</t>
-  </si>
-  <si>
-    <t>map</t>
-  </si>
-  <si>
-    <t>count</t>
-  </si>
-  <si>
-    <t>drop_while</t>
-  </si>
-  <si>
-    <t>each_with_index</t>
-  </si>
-  <si>
-    <t>each_with_object</t>
-  </si>
-  <si>
-    <t>max_by</t>
-  </si>
-  <si>
-    <t>each_cons (Part 1)</t>
-  </si>
-  <si>
-    <t>each_cons (Part 2)</t>
-  </si>
-  <si>
-    <t>Boolean Assertions</t>
-  </si>
-  <si>
-    <t>Equality Assertions</t>
-  </si>
-  <si>
-    <t>Nil Assertions</t>
-  </si>
-  <si>
-    <t>Empty Object Assertions</t>
-  </si>
-  <si>
-    <t>Included Object Assertions</t>
-  </si>
-  <si>
-    <t>Exception Assertions</t>
-  </si>
-  <si>
-    <t>Type Assertions</t>
-  </si>
-  <si>
-    <t>Kind Assertions</t>
-  </si>
-  <si>
-    <t>Same Object Assertions</t>
-  </si>
-  <si>
-    <t>Refutations</t>
-  </si>
-  <si>
-    <t>Listening Device</t>
-  </si>
-  <si>
-    <t>Text Analyzer - Sandwich Code</t>
-  </si>
-  <si>
-    <t>Passing Parameters Part 1</t>
-  </si>
-  <si>
-    <t>Passing Parameters Part 2</t>
-  </si>
-  <si>
-    <t>Passing Parameters Part 3</t>
-  </si>
-  <si>
-    <t>Method to Proc</t>
-  </si>
-  <si>
-    <t>Bubble Sort with Blocks</t>
-  </si>
-  <si>
-    <t>Classes to Test - Cash Register and Transaction</t>
-  </si>
-  <si>
-    <t>Setup the Test Class - Cash Register</t>
-  </si>
-  <si>
-    <t>Test Accept Money Method - Cash Register</t>
-  </si>
-  <si>
-    <t>Test Change Method - Cash Register</t>
-  </si>
-  <si>
-    <t>Test Give Receipt Method - Cash Register</t>
-  </si>
-  <si>
-    <t>Test Prompt For Payment Method- Transaction</t>
-  </si>
-  <si>
-    <t>Alter Prompt For Payment Method - Transaction</t>
-  </si>
-  <si>
-    <t>Swap Letters Sample Text and Starter File</t>
-  </si>
-  <si>
-    <t>Test swap method - Text</t>
-  </si>
-  <si>
-    <t>Test word_count method - Text</t>
-  </si>
-  <si>
-    <t>Internal vs External Iterators</t>
-  </si>
-  <si>
-    <t>Exploring Procs, Lambdas, and Blocks: Definition and Arity</t>
+    <t>Create a Database</t>
+  </si>
+  <si>
+    <t>Create a Table</t>
+  </si>
+  <si>
+    <t>Insert Data</t>
+  </si>
+  <si>
+    <t>Select Data</t>
+  </si>
+  <si>
+    <t>WHERE Clause</t>
+  </si>
+  <si>
+    <t>Update Data</t>
+  </si>
+  <si>
+    <t>Delete Data</t>
+  </si>
+  <si>
+    <t>Add Constraint</t>
+  </si>
+  <si>
+    <t>Drop Table</t>
+  </si>
+  <si>
+    <t>Drop Database</t>
   </si>
 </sst>
 </file>
@@ -664,20 +547,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF6CD41F-381F-429B-BA06-5048AE13F42A}">
   <dimension ref="A2:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -692,14 +575,14 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F2" t="str">
-        <f>D2&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E2," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_Enumerable_Class_Creation.rb</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <f>D2&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E2," ","_"),"?",""),"!",""),"(",""),")","")&amp;".sql"</f>
+        <v>1_Create_a_Database.sql</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>1</v>
       </c>
@@ -707,23 +590,23 @@
         <v>25</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F12" si="0">D3&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E3," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>2_Optional_Blocks.rb</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" ref="F3:F12" si="0">D3&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E3," ","_"),"?",""),"!",""),"(",""),")","")&amp;".sql"</f>
+        <v>2_Create_a_Table.sql</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>3_Find_Missing_Numbers.rb</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3_Insert_Data.sql</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>3</v>
       </c>
@@ -732,46 +615,46 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>4_Divisors.rb</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4_Select_Data.sql</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>5_Encrypted_Pioneers.rb</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5_WHERE_Clause.sql</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>6_Iterators:_True_for_Any.rb</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6_Update_Data.sql</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>7_Iterators:_True_for_All.rb</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7_Delete_Data.sql</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>7</v>
       </c>
@@ -780,22 +663,22 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>8_Iterators:_True_for_None.rb</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8_Add_Constraint.sql</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>9_Iterators:_True_for_One.rb</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9_Drop_Table.sql</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>9</v>
       </c>
@@ -804,20 +687,20 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>10_Count_Items.rb</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10_Drop_Database.sql</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>11_.rb</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>11_.sql</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -831,123 +714,103 @@
       <c r="D14" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" t="str">
         <f t="shared" ref="F14:F24" si="1">D14&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E14," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_From-To-Step_Sequence_Generator.rb</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1_.rb</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>2_Zipper.rb</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2_.rb</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
-        <v>3_map.rb</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3_.rb</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
-        <v>4_count.rb</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4_.rb</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
-        <v>5_drop_while.rb</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5_.rb</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
-        <v>6_each_with_index.rb</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6_.rb</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
-        <v>7_each_with_object.rb</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7_.rb</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="E21" s="2"/>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
-        <v>8_max_by.rb</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8_.rb</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="E22" s="1"/>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
-        <v>9_each_cons_Part_1.rb</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9_.rb</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
         <v>9</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
-        <v>10_each_cons_Part_2.rb</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10_.rb</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>10</v>
       </c>
@@ -957,12 +820,12 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" t="str">
         <f>A26&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B26,":","")," ","_"),"?",""),"!",""),"(",""),")","")</f>
@@ -971,123 +834,103 @@
       <c r="D26" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="E26" s="1"/>
       <c r="F26" t="str">
         <f t="shared" ref="F26:F36" si="2">D26&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E26," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_Boolean_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1_.rb</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" t="str">
         <f t="shared" si="2"/>
-        <v>2_Equality_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2_.rb</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>2</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>46</v>
-      </c>
+      <c r="E28" s="1"/>
       <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>3_Nil_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3_.rb</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>4_Empty_Object_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4_.rb</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="E30" s="3"/>
       <c r="F30" t="str">
         <f t="shared" si="2"/>
-        <v>5_Included_Object_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5_.rb</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" t="str">
         <f t="shared" si="2"/>
-        <v>6_Exception_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6_.rb</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>6</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" t="str">
         <f t="shared" si="2"/>
-        <v>7_Type_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7_.rb</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="E33" s="1"/>
       <c r="F33" t="str">
         <f t="shared" si="2"/>
-        <v>8_Kind_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8_.rb</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" t="str">
         <f t="shared" si="2"/>
-        <v>9_Same_Object_Assertions.rb</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9_.rb</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>10_Refutations.rb</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10_.rb</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>10</v>
       </c>
@@ -1097,7 +940,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1111,87 +954,73 @@
       <c r="D38" t="s">
         <v>0</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="E38" s="1"/>
       <c r="F38" t="str">
         <f t="shared" ref="F38:F48" si="3">D38&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E38," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_Listening_Device.rb</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1_.rb</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="E39" s="1"/>
       <c r="F39" t="str">
         <f t="shared" si="3"/>
-        <v>2_Text_Analyzer_-_Sandwich_Code.rb</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2_.rb</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="E40" s="1"/>
       <c r="F40" t="str">
         <f t="shared" si="3"/>
-        <v>3_Passing_Parameters_Part_1.rb</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3_.rb</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="E41" s="1"/>
       <c r="F41" t="str">
         <f t="shared" si="3"/>
-        <v>4_Passing_Parameters_Part_2.rb</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4_.rb</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D42" t="s">
         <v>4</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="E42" s="1"/>
       <c r="F42" t="str">
         <f t="shared" si="3"/>
-        <v>5_Passing_Parameters_Part_3.rb</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5_.rb</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="E43" s="2"/>
       <c r="F43" t="str">
         <f t="shared" si="3"/>
-        <v>6_Method_to_Proc.rb</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6_.rb</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
         <v>6</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="E44" s="1"/>
       <c r="F44" t="str">
         <f t="shared" si="3"/>
-        <v>7_Bubble_Sort_with_Blocks.rb</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7_.rb</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1030,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
         <v>8</v>
       </c>
@@ -1211,7 +1040,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
         <v>9</v>
       </c>
@@ -1221,7 +1050,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D48" t="s">
         <v>10</v>
       </c>
@@ -1231,12 +1060,12 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C50" t="str">
         <f>A50&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B50,":","")," ","_"),"?",""),"!",""),"(",""),")","")</f>
@@ -1245,123 +1074,103 @@
       <c r="D50" t="s">
         <v>0</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="E50" s="1"/>
       <c r="F50" t="str">
         <f t="shared" ref="F50:F60" si="4">D50&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E50," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_Classes_to_Test_-_Cash_Register_and_Transaction.rb</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1_.rb</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="E51" s="1"/>
       <c r="F51" t="str">
         <f t="shared" si="4"/>
-        <v>2_Setup_the_Test_Class_-_Cash_Register.rb</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2_.rb</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>2</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="E52" s="1"/>
       <c r="F52" t="str">
         <f t="shared" si="4"/>
-        <v>3_Test_Accept_Money_Method_-_Cash_Register.rb</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+        <v>3_.rb</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D53" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="E53" s="1"/>
       <c r="F53" t="str">
         <f t="shared" si="4"/>
-        <v>4_Test_Change_Method_-_Cash_Register.rb</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4_.rb</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
         <v>4</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="E54" s="1"/>
       <c r="F54" t="str">
         <f t="shared" si="4"/>
-        <v>5_Test_Give_Receipt_Method_-_Cash_Register.rb</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+        <v>5_.rb</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D55" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="E55" s="1"/>
       <c r="F55" t="str">
         <f t="shared" si="4"/>
-        <v>6_Test_Prompt_For_Payment_Method-_Transaction.rb</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6_.rb</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D56" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" t="str">
         <f t="shared" si="4"/>
-        <v>7_Alter_Prompt_For_Payment_Method_-_Transaction.rb</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+        <v>7_.rb</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D57" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="E57" s="1"/>
       <c r="F57" t="str">
         <f t="shared" si="4"/>
-        <v>8_Swap_Letters_Sample_Text_and_Starter_File.rb</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8_.rb</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D58" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="E58" s="1"/>
       <c r="F58" t="str">
         <f t="shared" si="4"/>
-        <v>9_Test_swap_method_-_Text.rb</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+        <v>9_.rb</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="E59" s="1"/>
       <c r="F59" t="str">
         <f t="shared" si="4"/>
-        <v>10_Test_word_count_method_-_Text.rb</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10_.rb</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60" t="s">
         <v>10</v>
       </c>
@@ -1371,7 +1180,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -1385,27 +1194,23 @@
       <c r="D62" t="s">
         <v>0</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="E62" s="1"/>
       <c r="F62" t="str">
         <f t="shared" ref="F62:F72" si="5">D62&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E62," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_Internal_vs_External_Iterators.rb</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1_.rb</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>1</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="E63" s="1"/>
       <c r="F63" t="str">
         <f t="shared" si="5"/>
-        <v>2_Exploring_Procs,_Lambdas,_and_Blocks:_Definition_and_Arity.rb</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2_.rb</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D64" t="s">
         <v>2</v>
       </c>
@@ -1415,7 +1220,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>3</v>
       </c>
@@ -1425,7 +1230,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>4</v>
       </c>
@@ -1435,7 +1240,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>5</v>
       </c>
@@ -1445,7 +1250,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D68" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1260,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D69" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +1270,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +1280,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>9</v>
       </c>
@@ -1485,7 +1290,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>10</v>
       </c>
@@ -1495,7 +1300,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -1509,27 +1314,23 @@
       <c r="D74" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="E74" s="1"/>
       <c r="F74" t="str">
         <f t="shared" ref="F74:F84" si="6">D74&amp;SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(E74," ","_"),"?",""),"!",""),"(",""),")","")&amp;".rb"</f>
-        <v>1_Internal_vs_External_Iterators.rb</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1_.rb</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>1</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="E75" s="1"/>
       <c r="F75" t="str">
         <f t="shared" si="6"/>
-        <v>2_Exploring_Procs,_Lambdas,_and_Blocks:_Definition_and_Arity.rb</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2_.rb</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1340,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>3</v>
       </c>
@@ -1549,7 +1350,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>4</v>
       </c>
@@ -1559,7 +1360,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
         <v>5</v>
       </c>
@@ -1569,7 +1370,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
         <v>6</v>
       </c>
@@ -1579,7 +1380,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D81" t="s">
         <v>7</v>
       </c>
@@ -1589,7 +1390,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D82" t="s">
         <v>8</v>
       </c>
@@ -1599,7 +1400,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D83" t="s">
         <v>9</v>
       </c>
@@ -1609,7 +1410,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1420,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -1639,7 +1440,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D87" t="s">
         <v>1</v>
       </c>
@@ -1649,7 +1450,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D88" t="s">
         <v>2</v>
       </c>
@@ -1659,7 +1460,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D89" t="s">
         <v>3</v>
       </c>
@@ -1669,7 +1470,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D90" t="s">
         <v>4</v>
       </c>
@@ -1679,7 +1480,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
         <v>5</v>
       </c>
@@ -1689,7 +1490,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
         <v>6</v>
       </c>
@@ -1699,7 +1500,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D93" t="s">
         <v>7</v>
       </c>
@@ -1709,7 +1510,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D94" t="s">
         <v>8</v>
       </c>
@@ -1719,7 +1520,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D95" t="s">
         <v>9</v>
       </c>
@@ -1729,7 +1530,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D96" t="s">
         <v>10</v>
       </c>
@@ -1739,8 +1540,8 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="97" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -1760,7 +1561,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D99" t="s">
         <v>1</v>
       </c>
@@ -1770,7 +1571,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D100" t="s">
         <v>2</v>
       </c>
@@ -1780,7 +1581,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D101" t="s">
         <v>3</v>
       </c>
@@ -1790,7 +1591,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
         <v>4</v>
       </c>
@@ -1800,7 +1601,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
         <v>5</v>
       </c>
@@ -1810,7 +1611,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
         <v>6</v>
       </c>
@@ -1820,7 +1621,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
         <v>7</v>
       </c>
@@ -1830,7 +1631,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D106" t="s">
         <v>8</v>
       </c>
@@ -1840,7 +1641,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D107" t="s">
         <v>9</v>
       </c>
@@ -1850,7 +1651,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D108" t="s">
         <v>10</v>
       </c>
@@ -1860,7 +1661,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>9</v>
       </c>
@@ -1880,7 +1681,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D111" t="s">
         <v>1</v>
       </c>
@@ -1890,7 +1691,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D112" t="s">
         <v>2</v>
       </c>
@@ -1900,7 +1701,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D113" t="s">
         <v>3</v>
       </c>
@@ -1910,7 +1711,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D114" t="s">
         <v>4</v>
       </c>
@@ -1920,7 +1721,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D115" t="s">
         <v>5</v>
       </c>
@@ -1930,7 +1731,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D116" t="s">
         <v>6</v>
       </c>
@@ -1940,7 +1741,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
         <v>7</v>
       </c>
@@ -1950,7 +1751,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D118" t="s">
         <v>8</v>
       </c>
@@ -1960,7 +1761,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
         <v>9</v>
       </c>
@@ -1970,7 +1771,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D120" t="s">
         <v>10</v>
       </c>
@@ -1980,7 +1781,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>10</v>
       </c>
@@ -2000,7 +1801,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
         <v>1</v>
       </c>
@@ -2010,7 +1811,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
         <v>2</v>
       </c>
@@ -2020,7 +1821,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
         <v>3</v>
       </c>
@@ -2030,7 +1831,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
         <v>4</v>
       </c>
@@ -2040,7 +1841,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
         <v>5</v>
       </c>
@@ -2050,7 +1851,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
         <v>6</v>
       </c>
@@ -2060,7 +1861,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
         <v>7</v>
       </c>
@@ -2070,7 +1871,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
         <v>8</v>
       </c>
@@ -2080,7 +1881,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
         <v>9</v>
       </c>
@@ -2090,7 +1891,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
         <v>10</v>
       </c>
@@ -2100,7 +1901,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="134" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -2120,7 +1921,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
         <v>1</v>
       </c>
@@ -2130,7 +1931,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
         <v>2</v>
       </c>
@@ -2140,7 +1941,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
         <v>3</v>
       </c>
@@ -2150,7 +1951,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
         <v>4</v>
       </c>
@@ -2160,7 +1961,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
         <v>5</v>
       </c>
@@ -2170,7 +1971,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
         <v>6</v>
       </c>
@@ -2180,7 +1981,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
         <v>7</v>
       </c>
@@ -2190,7 +1991,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
         <v>8</v>
       </c>
@@ -2200,7 +2001,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
         <v>9</v>
       </c>
@@ -2210,7 +2011,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
         <v>10</v>
       </c>
@@ -2220,7 +2021,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>12</v>
       </c>
@@ -2240,7 +2041,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
         <v>1</v>
       </c>
@@ -2250,7 +2051,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
         <v>2</v>
       </c>
@@ -2260,7 +2061,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
         <v>3</v>
       </c>
@@ -2270,7 +2071,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
         <v>4</v>
       </c>
@@ -2280,7 +2081,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
         <v>5</v>
       </c>
@@ -2290,7 +2091,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
         <v>6</v>
       </c>
@@ -2300,7 +2101,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
         <v>7</v>
       </c>
@@ -2310,7 +2111,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
         <v>8</v>
       </c>
@@ -2320,7 +2121,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
         <v>9</v>
       </c>
@@ -2330,7 +2131,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
         <v>10</v>
       </c>
@@ -2340,7 +2141,7 @@
         <v>11_.rb</v>
       </c>
     </row>
-    <row r="158" spans="1:6" ht="31" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>13</v>
       </c>
@@ -2360,7 +2161,7 @@
         <v>1_.rb</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
         <v>1</v>
       </c>
@@ -2370,7 +2171,7 @@
         <v>2_.rb</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
         <v>2</v>
       </c>
@@ -2380,7 +2181,7 @@
         <v>3_.rb</v>
       </c>
     </row>
-    <row r="161" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
         <v>3</v>
       </c>
@@ -2390,7 +2191,7 @@
         <v>4_.rb</v>
       </c>
     </row>
-    <row r="162" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
         <v>4</v>
       </c>
@@ -2400,7 +2201,7 @@
         <v>5_.rb</v>
       </c>
     </row>
-    <row r="163" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
         <v>5</v>
       </c>
@@ -2410,7 +2211,7 @@
         <v>6_.rb</v>
       </c>
     </row>
-    <row r="164" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
         <v>6</v>
       </c>
@@ -2420,7 +2221,7 @@
         <v>7_.rb</v>
       </c>
     </row>
-    <row r="165" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
         <v>7</v>
       </c>
@@ -2430,7 +2231,7 @@
         <v>8_.rb</v>
       </c>
     </row>
-    <row r="166" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D166" t="s">
         <v>8</v>
       </c>
@@ -2440,7 +2241,7 @@
         <v>9_.rb</v>
       </c>
     </row>
-    <row r="167" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
         <v>9</v>
       </c>
@@ -2450,7 +2251,7 @@
         <v>10_.rb</v>
       </c>
     </row>
-    <row r="168" spans="4:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
         <v>10</v>
       </c>
@@ -2464,57 +2265,23 @@
   <hyperlinks>
     <hyperlink ref="B74" r:id="rId1" display="https://launchschool.com/exercise_sets/e0cc58f8" xr:uid="{A9B2050A-EC3E-439E-902E-401D4004127E}"/>
     <hyperlink ref="B86" r:id="rId2" display="https://launchschool.com/exercise_sets/5e5f2772" xr:uid="{7D876CFD-ACBD-4D15-A3DE-40802E2D0AE3}"/>
-    <hyperlink ref="E2" r:id="rId3" display="https://launchschool.com/exercises/583a1348" xr:uid="{31FD3A49-A0D5-41F3-BD5B-C6D9209A8EE5}"/>
-    <hyperlink ref="B14" r:id="rId4" display="https://launchschool.com/exercise_sets/3ea9ead7" xr:uid="{014E6063-FF67-4595-808A-DD09B5BB4204}"/>
-    <hyperlink ref="B26" r:id="rId5" display="https://launchschool.com/exercise_sets/94a0efb0" xr:uid="{FAF9C4D8-DA94-459C-9D32-69FDA2078EDA}"/>
-    <hyperlink ref="B38" r:id="rId6" display="https://launchschool.com/exercise_sets/f3f8b728" xr:uid="{22ECB839-31BF-4780-B06D-ADA751ACDF16}"/>
-    <hyperlink ref="B50" r:id="rId7" display="https://launchschool.com/exercise_sets/c8bbfe96" xr:uid="{087200F4-776A-4ABC-A307-F3D7DCA533A5}"/>
-    <hyperlink ref="B62" r:id="rId8" display="https://launchschool.com/exercise_sets/10775edd" xr:uid="{0C3CFEC6-0CF6-488F-8AC5-6D6F5917B515}"/>
-    <hyperlink ref="E3" r:id="rId9" display="https://launchschool.com/exercises/1e706bb0" xr:uid="{9F8D57F3-6508-422F-B745-5A2013BBE1D4}"/>
-    <hyperlink ref="E4" r:id="rId10" display="https://launchschool.com/exercises/a0a4a3d4" xr:uid="{A8702A2F-F55A-48F6-8BCC-E710C31A479D}"/>
-    <hyperlink ref="E5" r:id="rId11" display="https://launchschool.com/exercises/8b99f281" xr:uid="{0876D9DF-AF2B-4351-A73C-C39AEDE1B028}"/>
-    <hyperlink ref="E6" r:id="rId12" display="https://launchschool.com/exercises/6990f3dc" xr:uid="{2DE34EAA-F1FA-426D-B1B5-0D59EC0A6B5D}"/>
-    <hyperlink ref="E7" r:id="rId13" display="https://launchschool.com/exercises/944b8310" xr:uid="{E0A7FB3D-C777-4316-A04E-748CB6EDBCAE}"/>
-    <hyperlink ref="E8" r:id="rId14" display="https://launchschool.com/exercises/9c2b1d27" xr:uid="{0CEC0F6A-9F18-4763-A889-87C87DBA3D7F}"/>
-    <hyperlink ref="E9" r:id="rId15" display="https://launchschool.com/exercises/11204cc9" xr:uid="{42109F54-A955-42E0-AC31-A852AA364931}"/>
-    <hyperlink ref="E10" r:id="rId16" display="https://launchschool.com/exercises/ea073d36" xr:uid="{F9734E2A-4A04-4451-8251-D12D62AB14DD}"/>
-    <hyperlink ref="E11" r:id="rId17" display="https://launchschool.com/exercises/1318cb92" xr:uid="{F1433EF6-18E1-45AD-9871-FFD24E85ADDE}"/>
-    <hyperlink ref="E14" r:id="rId18" display="https://launchschool.com/exercises/ec8dd514" xr:uid="{0818C16F-CCBF-41A9-AA6F-E1DC923442B5}"/>
-    <hyperlink ref="E15" r:id="rId19" display="https://launchschool.com/exercises/7c6be14d" xr:uid="{E52205FF-8D3A-4D85-A595-643016174553}"/>
-    <hyperlink ref="E16" r:id="rId20" display="https://launchschool.com/exercises/8341f1f1" xr:uid="{CEF2F9B1-70BB-4542-A267-17EC84029226}"/>
-    <hyperlink ref="E26" r:id="rId21" display="https://launchschool.com/exercises/66216db8" xr:uid="{0BE6025F-1CFD-410D-AC9F-702836B8FFD9}"/>
-    <hyperlink ref="E27" r:id="rId22" display="https://launchschool.com/exercises/d69b88d6" xr:uid="{52369875-4445-423B-8821-16DB41D6D099}"/>
-    <hyperlink ref="E28" r:id="rId23" display="https://launchschool.com/exercises/e1183a98" xr:uid="{F3530559-4EC4-4A54-8843-5B45677A9D3E}"/>
-    <hyperlink ref="E29" r:id="rId24" display="https://launchschool.com/exercises/eaa85d07" xr:uid="{31464AA0-A56C-4243-8FEE-A7CF60C05621}"/>
-    <hyperlink ref="E30" r:id="rId25" display="https://launchschool.com/exercises/12b78daf" xr:uid="{18F45D43-0C29-4D67-9618-7DA29A1B71C6}"/>
-    <hyperlink ref="E31" r:id="rId26" display="https://launchschool.com/exercises/82b73047" xr:uid="{FB86B878-A38B-407A-841D-DC4E03F5C814}"/>
-    <hyperlink ref="E32" r:id="rId27" display="https://launchschool.com/exercises/92e1ef71" xr:uid="{4EBABAFB-B13A-462B-9151-CE15F76351C7}"/>
-    <hyperlink ref="E33" r:id="rId28" display="https://launchschool.com/exercises/098fba0b" xr:uid="{C9BEADA7-815A-4446-B0B6-5EE6B446AF81}"/>
-    <hyperlink ref="E34" r:id="rId29" display="https://launchschool.com/exercises/9eed2942" xr:uid="{05C7FB3F-DF52-4E7E-9992-37F34D28FA90}"/>
-    <hyperlink ref="E35" r:id="rId30" display="https://launchschool.com/exercises/4ac8e502" xr:uid="{F0E547E3-83A1-409E-936C-E6AC39FA72AF}"/>
-    <hyperlink ref="E38" r:id="rId31" display="https://launchschool.com/exercises/56a87411" xr:uid="{CB8BD403-2020-4874-9D69-BF89F51871B4}"/>
-    <hyperlink ref="E39" r:id="rId32" display="https://launchschool.com/exercises/c618c0e4" xr:uid="{A61A2B88-C6F7-4A65-97E7-663107CE70F4}"/>
-    <hyperlink ref="E40" r:id="rId33" display="https://launchschool.com/exercises/c7f39d55" xr:uid="{811D71C6-3D49-4DEB-ABF9-0E2F1F186016}"/>
-    <hyperlink ref="E41" r:id="rId34" display="https://launchschool.com/exercises/8621919c" xr:uid="{649991BB-B44A-4ACD-B764-FC88D7645A51}"/>
-    <hyperlink ref="E42" r:id="rId35" display="https://launchschool.com/exercises/c9181c33" xr:uid="{2579491C-7362-4C65-8F26-21A07F0830B7}"/>
-    <hyperlink ref="E43" r:id="rId36" display="https://launchschool.com/exercises/ecdb2b22" xr:uid="{DC546216-C3DE-4C8F-AD5D-7A62342669C9}"/>
-    <hyperlink ref="E44" r:id="rId37" display="https://launchschool.com/exercises/8a0837d6" xr:uid="{F99ADC73-50EF-4239-A214-40C9A0587ABF}"/>
-    <hyperlink ref="E50" r:id="rId38" display="https://launchschool.com/exercises/0af19f30" xr:uid="{70F52219-8901-4039-A575-27672307F7FD}"/>
-    <hyperlink ref="E51" r:id="rId39" display="https://launchschool.com/exercises/82de3f03" xr:uid="{3CE11E25-CF40-4C4F-90DF-8BECC89A4CEA}"/>
-    <hyperlink ref="E52" r:id="rId40" display="https://launchschool.com/exercises/acc0412a" xr:uid="{3B2B8E02-6E8F-4E13-894C-80BE39CEEA56}"/>
-    <hyperlink ref="E53" r:id="rId41" display="https://launchschool.com/exercises/4c36c285" xr:uid="{0C963815-4B66-4E03-8465-1CB826596E46}"/>
-    <hyperlink ref="E54" r:id="rId42" display="https://launchschool.com/exercises/8cf7a4e3" xr:uid="{F1BFAEAD-556A-48E0-877D-E6E8D52A1C25}"/>
-    <hyperlink ref="E55" r:id="rId43" display="https://launchschool.com/exercises/64799839" xr:uid="{B4FD0494-A451-423E-9B2B-42E86F8F7503}"/>
-    <hyperlink ref="E56" r:id="rId44" display="https://launchschool.com/exercises/e2b66911" xr:uid="{A2BAAB47-9707-4611-8B7B-A906CD9E0C68}"/>
-    <hyperlink ref="E57" r:id="rId45" display="https://launchschool.com/exercises/20ec4425" xr:uid="{8936B52F-BE06-49B8-8E26-138C0694530D}"/>
-    <hyperlink ref="E58" r:id="rId46" display="https://launchschool.com/exercises/82427de8" xr:uid="{AEEE429C-BDDF-4D12-A360-EF459DE89ABE}"/>
-    <hyperlink ref="E59" r:id="rId47" display="https://launchschool.com/exercises/530e4c03" xr:uid="{52D928F4-102B-4130-A073-ABA1ABE552C0}"/>
-    <hyperlink ref="E74" r:id="rId48" display="https://launchschool.com/exercises/0b6294cb" xr:uid="{5DF58641-D338-4B99-A185-F478C79CB72F}"/>
-    <hyperlink ref="E75" r:id="rId49" display="https://launchschool.com/exercises/753d0323" xr:uid="{B49880D9-DEE5-4A1A-B59B-ED39BA336E3C}"/>
-    <hyperlink ref="E62" r:id="rId50" display="https://launchschool.com/exercises/0b6294cb" xr:uid="{B88383EA-7B28-4F78-93DB-BBA56AD57844}"/>
-    <hyperlink ref="E63" r:id="rId51" display="https://launchschool.com/exercises/753d0323" xr:uid="{35B02EFD-68F6-4C57-A14C-57C890C272E3}"/>
+    <hyperlink ref="B14" r:id="rId3" display="https://launchschool.com/exercise_sets/3ea9ead7" xr:uid="{014E6063-FF67-4595-808A-DD09B5BB4204}"/>
+    <hyperlink ref="B26" r:id="rId4" display="https://launchschool.com/exercise_sets/94a0efb0" xr:uid="{FAF9C4D8-DA94-459C-9D32-69FDA2078EDA}"/>
+    <hyperlink ref="B38" r:id="rId5" display="https://launchschool.com/exercise_sets/f3f8b728" xr:uid="{22ECB839-31BF-4780-B06D-ADA751ACDF16}"/>
+    <hyperlink ref="B50" r:id="rId6" display="https://launchschool.com/exercise_sets/c8bbfe96" xr:uid="{087200F4-776A-4ABC-A307-F3D7DCA533A5}"/>
+    <hyperlink ref="B62" r:id="rId7" display="https://launchschool.com/exercise_sets/10775edd" xr:uid="{0C3CFEC6-0CF6-488F-8AC5-6D6F5917B515}"/>
+    <hyperlink ref="E2" r:id="rId8" display="https://launchschool.com/exercises/43313d09" xr:uid="{7FAB21B9-96DD-4EB6-949A-8A6B072931D3}"/>
+    <hyperlink ref="E3" r:id="rId9" display="https://launchschool.com/exercises/2ac78074" xr:uid="{2C8F8C56-BEB7-4E0F-ABC3-07B2484CE9FD}"/>
+    <hyperlink ref="E4" r:id="rId10" display="https://launchschool.com/exercises/b06c9ec4" xr:uid="{52FAD4C9-B7F1-4D69-8314-706AA42833CB}"/>
+    <hyperlink ref="E5" r:id="rId11" display="https://launchschool.com/exercises/35962964" xr:uid="{5A47AD7A-9B85-4CD6-A93F-17F2F7EF9BD0}"/>
+    <hyperlink ref="E6" r:id="rId12" display="https://launchschool.com/exercises/f7ff3f4e" xr:uid="{A4B0D499-861D-436E-A78D-9F60284D571F}"/>
+    <hyperlink ref="E7" r:id="rId13" display="https://launchschool.com/exercises/3b5163ba" xr:uid="{C3609073-9EE5-4582-A00F-6F64E6E81A10}"/>
+    <hyperlink ref="E8" r:id="rId14" display="https://launchschool.com/exercises/722ac41c" xr:uid="{278113DD-EA76-4476-8760-062D090E856B}"/>
+    <hyperlink ref="E9" r:id="rId15" display="https://launchschool.com/exercises/d176489a" xr:uid="{D9F9E070-64F1-4ECB-8741-B856F2F78530}"/>
+    <hyperlink ref="E10" r:id="rId16" display="https://launchschool.com/exercises/c5e3018b" xr:uid="{B3FD7AAD-5A88-444D-9FE9-156DD5880E10}"/>
+    <hyperlink ref="E11" r:id="rId17" display="https://launchschool.com/exercises/f700f999" xr:uid="{24651472-1CAE-465E-B868-187EA28B1C3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId52"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>